<commit_message>
Addedd Verify data tab for Manager - Bart
</commit_message>
<xml_diff>
--- a/WeatherApp/Resources/Raw/Metadata.xlsx
+++ b/WeatherApp/Resources/Raw/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10303"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livenapierac-my.sharepoint.com/personal/b_davison_napier_ac_uk/Documents/Modules/SET09102/2024-25/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Documents/SE_class/WeatherApp/WeatherApp/Resources/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{8F183D94-9855-1144-8ABD-E006D78D5089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B653FA92-BECD-F04B-AAA6-F8D4C0222DB6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96B3405-6A58-CF4D-A403-483E0FA7DEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="5380" windowWidth="27240" windowHeight="16440" xr2:uid="{4ED62BD8-9A4B-3549-B4A0-F1C3BE0A5B45}"/>
+    <workbookView xWindow="4440" yWindow="2680" windowWidth="24960" windowHeight="16440" xr2:uid="{4ED62BD8-9A4B-3549-B4A0-F1C3BE0A5B45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -638,7 +638,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,6 +970,9 @@
       <c r="F11" t="s">
         <v>50</v>
       </c>
+      <c r="G11">
+        <v>28</v>
+      </c>
       <c r="I11" t="s">
         <v>66</v>
       </c>
@@ -993,6 +996,9 @@
       <c r="F12" t="s">
         <v>50</v>
       </c>
+      <c r="G12">
+        <v>26</v>
+      </c>
       <c r="I12" t="s">
         <v>66</v>
       </c>
@@ -1016,6 +1022,9 @@
       <c r="F13" t="s">
         <v>50</v>
       </c>
+      <c r="G13">
+        <v>45</v>
+      </c>
       <c r="I13" t="s">
         <v>68</v>
       </c>
@@ -1038,6 +1047,9 @@
       </c>
       <c r="F14" t="s">
         <v>50</v>
+      </c>
+      <c r="G14">
+        <v>48</v>
       </c>
       <c r="I14" t="s">
         <v>68</v>

</xml_diff>